<commit_message>
Cruise and Planning Fee
</commit_message>
<xml_diff>
--- a/ClassLibrary1/TestData/TestData.xlsx
+++ b/ClassLibrary1/TestData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="6216" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="6210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>lax</t>
-  </si>
-  <si>
-    <t>LAX</t>
   </si>
 </sst>
 </file>
@@ -543,14 +540,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +558,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -569,7 +566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -593,13 +590,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -607,15 +604,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -623,7 +620,7 @@
         <v>42995</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -631,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -639,7 +636,7 @@
         <v>42999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
     </row>
   </sheetData>
@@ -656,13 +653,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -670,7 +667,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -678,7 +675,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -686,7 +683,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -694,7 +691,7 @@
         <v>42964</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -702,7 +699,7 @@
         <v>42966</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -710,7 +707,7 @@
         <v>42968</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -728,13 +725,13 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -755,13 +752,13 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -769,7 +766,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -777,7 +774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -785,7 +782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -793,7 +790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -801,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -809,7 +806,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -830,13 +827,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -844,7 +841,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -852,7 +849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -860,7 +857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -868,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -876,7 +873,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -884,7 +881,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -892,7 +889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -900,7 +897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -908,7 +905,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -916,7 +913,7 @@
         <v>4677</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>

</xml_diff>